<commit_message>
removed Dussa, Reese until they actually submit text ;-) Sorted authors in alphabetical order by last name
</commit_message>
<xml_diff>
--- a/src/table_tls.xlsx
+++ b/src/table_tls.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="1" r:id="rId1"/>
     <sheet name="Browsers" sheetId="2" r:id="rId2"/>
     <sheet name="Suggestions" sheetId="3" r:id="rId3"/>
+    <sheet name="Blatt1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Elliptic_curve_cipher_suites_TL" localSheetId="1">Browsers!$F$14</definedName>
+    <definedName name="foo" localSheetId="3">Blatt1!$A$2:$F$38</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,8 +25,25 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="foo.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="duracell:Users:aaron:Desktop:work:nic.at:projects:ACH:ach-master:src:foo.csv" tab="0" semicolon="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="814">
   <si>
     <t>RFC2246 - TLS1.0</t>
   </si>
@@ -2328,13 +2347,151 @@
   </si>
   <si>
     <t>DHE-DSS-CAMELLIA256-SHA</t>
+  </si>
+  <si>
+    <t>TLS_EMPTY_RENEGOTIATION_INFO_SCSV</t>
+  </si>
+  <si>
+    <t>(0xff)	-</t>
+  </si>
+  <si>
+    <t>(0xc00a)</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Secrecy	256</t>
+  </si>
+  <si>
+    <t>(0xc014)</t>
+  </si>
+  <si>
+    <t>(0x88)</t>
+  </si>
+  <si>
+    <t>(0x87)</t>
+  </si>
+  <si>
+    <t>Secrecy*	256</t>
+  </si>
+  <si>
+    <t>(0x39)</t>
+  </si>
+  <si>
+    <t>(0x38)</t>
+  </si>
+  <si>
+    <t>(0xc00f)	256</t>
+  </si>
+  <si>
+    <t>(0xc005)	256</t>
+  </si>
+  <si>
+    <t>(0x84)	256</t>
+  </si>
+  <si>
+    <t>(0x35)	256</t>
+  </si>
+  <si>
+    <t>(0xc007)</t>
+  </si>
+  <si>
+    <t>Secrecy	128</t>
+  </si>
+  <si>
+    <t>(0xc009)</t>
+  </si>
+  <si>
+    <t>(0xc011)</t>
+  </si>
+  <si>
+    <t>(0xc013)</t>
+  </si>
+  <si>
+    <t>(0x45)</t>
+  </si>
+  <si>
+    <t>(0x44)</t>
+  </si>
+  <si>
+    <t>Secrecy*	128</t>
+  </si>
+  <si>
+    <t>(0x33)</t>
+  </si>
+  <si>
+    <t>(0x32)</t>
+  </si>
+  <si>
+    <t>(0xc00c)	128</t>
+  </si>
+  <si>
+    <t>(0xc00e)	128</t>
+  </si>
+  <si>
+    <t>(0xc002)	128</t>
+  </si>
+  <si>
+    <t>(0xc004)	128</t>
+  </si>
+  <si>
+    <t>(0x96)	128</t>
+  </si>
+  <si>
+    <t>(0x41)	128</t>
+  </si>
+  <si>
+    <t>(0x5)	128</t>
+  </si>
+  <si>
+    <t>(0x4)	128</t>
+  </si>
+  <si>
+    <t>(0x2f)	128</t>
+  </si>
+  <si>
+    <t>(0xc008)</t>
+  </si>
+  <si>
+    <t>Secrecy	168</t>
+  </si>
+  <si>
+    <t>(0xc012)</t>
+  </si>
+  <si>
+    <t>(0x16)</t>
+  </si>
+  <si>
+    <t>(0x13)</t>
+  </si>
+  <si>
+    <t>Secrecy*	168</t>
+  </si>
+  <si>
+    <t>(0xc00d)	168</t>
+  </si>
+  <si>
+    <t>(0xc003)	168</t>
+  </si>
+  <si>
+    <t>SSL_RSA_FIPS_WITH_3DES_EDE_CBC_SHA</t>
+  </si>
+  <si>
+    <t>(0xfeff)	168</t>
+  </si>
+  <si>
+    <t>(0xa)	168</t>
+  </si>
+  <si>
+    <t>Firefox 10.0.12 ESR / Win 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2383,6 +2540,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="27"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3019,7 +3182,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3032,14 +3195,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="585">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -3633,6 +3797,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="foo" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
   <a:themeElements>
@@ -3957,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AP78"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AD26" sqref="AD26"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3988,82 +4156,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12" t="s">
+      <c r="U1" s="14"/>
+      <c r="V1" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12" t="s">
+      <c r="W1" s="14"/>
+      <c r="X1" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12" t="s">
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12" t="s">
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12" t="s">
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12" t="s">
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14" t="s">
         <v>665</v>
       </c>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12" t="s">
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12" t="s">
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14" t="s">
         <v>543</v>
       </c>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12" t="s">
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14" t="s">
         <v>628</v>
       </c>
-      <c r="AM1" s="12"/>
+      <c r="AM1" s="14"/>
       <c r="AN1" s="3" t="s">
         <v>661</v>
       </c>
@@ -7062,12 +7230,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="N1:O1"/>
@@ -7081,6 +7243,12 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7096,8 +7264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7229,7 +7397,7 @@
       <c r="G10" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>753</v>
       </c>
     </row>
@@ -7255,7 +7423,7 @@
       <c r="G11" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>753</v>
       </c>
     </row>
@@ -7281,7 +7449,7 @@
       <c r="G12" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>755</v>
       </c>
     </row>
@@ -7307,7 +7475,7 @@
       <c r="G13" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>754</v>
       </c>
     </row>
@@ -7333,7 +7501,7 @@
       <c r="G14" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>754</v>
       </c>
     </row>
@@ -7359,7 +7527,7 @@
       <c r="G15" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="13" t="s">
         <v>756</v>
       </c>
     </row>
@@ -7385,7 +7553,7 @@
       <c r="G16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>758</v>
       </c>
     </row>
@@ -7411,7 +7579,7 @@
       <c r="G17" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="13" t="s">
         <v>757</v>
       </c>
     </row>
@@ -7437,7 +7605,7 @@
       <c r="G18" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>757</v>
       </c>
     </row>
@@ -7719,7 +7887,7 @@
   <dimension ref="A3:M26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B4" sqref="B4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8074,4 +8242,431 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31">
+      <c r="A1" s="16" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>768</v>
+      </c>
+      <c r="B2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>770</v>
+      </c>
+      <c r="E3" t="s">
+        <v>771</v>
+      </c>
+      <c r="F3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>773</v>
+      </c>
+      <c r="E4" t="s">
+        <v>771</v>
+      </c>
+      <c r="F4" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>774</v>
+      </c>
+      <c r="E5" t="s">
+        <v>771</v>
+      </c>
+      <c r="F5" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>775</v>
+      </c>
+      <c r="E6" t="s">
+        <v>771</v>
+      </c>
+      <c r="F6" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E7" t="s">
+        <v>771</v>
+      </c>
+      <c r="F7" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>778</v>
+      </c>
+      <c r="E8" t="s">
+        <v>771</v>
+      </c>
+      <c r="F8" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>783</v>
+      </c>
+      <c r="E13" t="s">
+        <v>771</v>
+      </c>
+      <c r="F13" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" t="s">
+        <v>785</v>
+      </c>
+      <c r="E14" t="s">
+        <v>771</v>
+      </c>
+      <c r="F14" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" t="s">
+        <v>786</v>
+      </c>
+      <c r="E15" t="s">
+        <v>771</v>
+      </c>
+      <c r="F15" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>787</v>
+      </c>
+      <c r="E16" t="s">
+        <v>771</v>
+      </c>
+      <c r="F16" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>788</v>
+      </c>
+      <c r="E17" t="s">
+        <v>771</v>
+      </c>
+      <c r="F17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>789</v>
+      </c>
+      <c r="E18" t="s">
+        <v>771</v>
+      </c>
+      <c r="F18" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>791</v>
+      </c>
+      <c r="E19" t="s">
+        <v>771</v>
+      </c>
+      <c r="F19" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>792</v>
+      </c>
+      <c r="E20" t="s">
+        <v>771</v>
+      </c>
+      <c r="F20" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" t="s">
+        <v>802</v>
+      </c>
+      <c r="E30" t="s">
+        <v>771</v>
+      </c>
+      <c r="F30" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" t="s">
+        <v>804</v>
+      </c>
+      <c r="E31" t="s">
+        <v>771</v>
+      </c>
+      <c r="F31" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>805</v>
+      </c>
+      <c r="E32" t="s">
+        <v>771</v>
+      </c>
+      <c r="F32" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>806</v>
+      </c>
+      <c r="E33" t="s">
+        <v>771</v>
+      </c>
+      <c r="F33" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>184</v>
+      </c>
+      <c r="B35" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>810</v>
+      </c>
+      <c r="B36" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>812</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>